<commit_message>
Auto-committed on 2021/12/17 週五
Former-commit-id: b312e98ce1c048758c2a649e502a859a59dec888
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/AcReceivable.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/AcReceivable.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\SKL\DB\GenTables\L6-共同作業\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\DB\GenTables\L6-共同作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6AEA38-4C46-417E-9DD1-6538AD36ED15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">資料轉換!$A$1:$Q$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="394">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1547,10 +1548,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>FacmNo ASC</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>CustNo ASC,FacmNo ASC</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -1596,11 +1593,26 @@
 5.另收欠款</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>FacmNo ASC,RvNo DESC</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>useL2r58Eq</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FacmNo ASC,RvNo Asc</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CustNo = ,AND FacmNo = ,AND AcctFlag &gt;= ,AND AcctFlag &lt;= ,AND RvNo %</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19">
     <font>
       <sz val="12"/>
@@ -2332,9 +2344,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 2" xfId="1"/>
-    <cellStyle name="一般 2 2" xfId="3"/>
-    <cellStyle name="一般_CopyBook" xfId="2"/>
+    <cellStyle name="一般 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="一般 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="一般_CopyBook" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2491,6 +2503,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2526,6 +2555,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2701,7 +2747,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -2843,10 +2889,10 @@
         <v>86</v>
       </c>
       <c r="C9" s="42" t="s">
+        <v>386</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>387</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>388</v>
       </c>
       <c r="E9" s="43">
         <v>3</v>
@@ -2917,7 +2963,7 @@
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="28" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -3079,7 +3125,7 @@
         <v>76</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>77</v>
@@ -3089,7 +3135,7 @@
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="37" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -3507,12 +3553,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -3597,7 +3643,7 @@
         <v>157</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3608,7 +3654,7 @@
         <v>183</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="32.4">
@@ -3641,7 +3687,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="37.200000000000003" customHeight="1">
@@ -3685,7 +3731,18 @@
         <v>381</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>382</v>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -3696,10 +3753,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -3832,7 +3889,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4429,7 +4486,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -5371,7 +5428,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q1"/>
+  <autoFilter ref="A1:Q1" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Auto-committed on 2021/12/20 週一
Former-commit-id: 1040746f074ee05c58c2d6690360832154b2caf1
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/AcReceivable.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/AcReceivable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\DB\GenTables\L6-共同作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6AEA38-4C46-417E-9DD1-6538AD36ED15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C23EE93-B7BF-4DB2-9D9B-E7B2F8DA437A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="396">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1607,6 +1607,14 @@
   </si>
   <si>
     <t>CustNo = ,AND FacmNo = ,AND AcctFlag &gt;= ,AND AcctFlag &lt;= ,AND RvNo %</t>
+  </si>
+  <si>
+    <t>useBs902Eq</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CustNo &gt;= ,AND CustNo &lt;= ,AND ClsFlag = ,AND ReceivableFlag = ,AND RvNo %</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3554,11 +3562,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -3743,6 +3751,17 @@
       </c>
       <c r="C16" s="1" t="s">
         <v>392</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2022/01/18 週二
Former-commit-id: 5069afc59837164bce7dbeb2b5297dfea2525ccd
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/AcReceivable.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/AcReceivable.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\DB\GenTables\L6-共同作業\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\SKL\DB\GenTables\L6-共同作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C23EE93-B7BF-4DB2-9D9B-E7B2F8DA437A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">資料轉換!$A$1:$Q$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="397">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1042,10 +1041,6 @@
   </si>
   <si>
     <t>轉換規則</t>
-    <phoneticPr fontId="17" type="noConversion"/>
-  </si>
-  <si>
-    <t>InsuStartDate保險起日</t>
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
@@ -1616,11 +1611,19 @@
     <t>CustNo &gt;= ,AND CustNo &lt;= ,AND ClsFlag = ,AND ReceivableFlag = ,AND RvNo %</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>火險單年月InsuYearMonth+01</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>火險單年月InsuYearMonth+01</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19">
     <font>
       <sz val="12"/>
@@ -2352,9 +2355,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="一般 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="一般_CopyBook" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="一般 2" xfId="1"/>
+    <cellStyle name="一般 2 2" xfId="3"/>
+    <cellStyle name="一般_CopyBook" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2511,23 +2514,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2563,23 +2549,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2755,7 +2724,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -2897,10 +2866,10 @@
         <v>86</v>
       </c>
       <c r="C9" s="42" t="s">
+        <v>385</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>386</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>387</v>
       </c>
       <c r="E9" s="43">
         <v>3</v>
@@ -2971,7 +2940,7 @@
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -3121,7 +3090,7 @@
       </c>
       <c r="F19" s="33"/>
       <c r="G19" s="34" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="35" customFormat="1" ht="81">
@@ -3133,7 +3102,7 @@
         <v>76</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>77</v>
@@ -3143,7 +3112,7 @@
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="37" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -3264,10 +3233,10 @@
         <v>18</v>
       </c>
       <c r="B26" s="95" t="s">
+        <v>369</v>
+      </c>
+      <c r="C26" s="96" t="s">
         <v>370</v>
-      </c>
-      <c r="C26" s="96" t="s">
-        <v>371</v>
       </c>
       <c r="D26" s="96" t="s">
         <v>85</v>
@@ -3277,7 +3246,7 @@
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="98" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -3299,7 +3268,7 @@
       </c>
       <c r="F27" s="23"/>
       <c r="G27" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -3374,7 +3343,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="42" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C31" s="42" t="s">
         <v>14</v>
@@ -3561,10 +3530,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
@@ -3651,7 +3620,7 @@
         <v>157</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3662,7 +3631,7 @@
         <v>183</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="32.4">
@@ -3695,15 +3664,15 @@
         <v>208</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="37.200000000000003" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>197</v>
@@ -3711,10 +3680,10 @@
     </row>
     <row r="13" spans="1:3" ht="32.4">
       <c r="A13" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>193</v>
@@ -3722,10 +3691,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>184</v>
@@ -3733,32 +3702,32 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>381</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>391</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>395</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>184</v>
@@ -3772,7 +3741,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3822,7 +3791,7 @@
         <v>54</v>
       </c>
       <c r="I5" s="94" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="35" customFormat="1" ht="164.4" customHeight="1">
@@ -3830,7 +3799,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D6" s="74" t="s">
         <v>179</v>
@@ -3843,10 +3812,10 @@
       </c>
       <c r="G6" s="32"/>
       <c r="H6" s="34" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I6" s="35" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="35" customFormat="1" ht="78" customHeight="1">
@@ -3854,10 +3823,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="34" t="s">
+        <v>353</v>
+      </c>
+      <c r="D7" s="34" t="s">
         <v>354</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>355</v>
       </c>
       <c r="E7" s="32" t="s">
         <v>85</v>
@@ -3867,10 +3836,10 @@
       </c>
       <c r="G7" s="32"/>
       <c r="H7" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="I7" s="35" t="s">
         <v>356</v>
-      </c>
-      <c r="I7" s="35" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="35" customFormat="1" ht="24.6" customHeight="1">
@@ -3878,10 +3847,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>12</v>
@@ -3891,10 +3860,10 @@
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="34" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3908,7 +3877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4505,12 +4474,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.2"/>
@@ -4530,7 +4499,7 @@
     <col min="13" max="13" width="21.77734375" style="79" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.21875" style="79" customWidth="1"/>
     <col min="15" max="15" width="8" style="79" customWidth="1"/>
-    <col min="16" max="16" width="25.109375" style="79" customWidth="1"/>
+    <col min="16" max="16" width="31.44140625" style="79" customWidth="1"/>
     <col min="17" max="17" width="53" style="79" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="8.88671875" style="79"/>
   </cols>
@@ -4549,7 +4518,7 @@
         <v>265</v>
       </c>
       <c r="E1" s="88" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F1" s="78" t="s">
         <v>247</v>
@@ -4558,7 +4527,7 @@
         <v>248</v>
       </c>
       <c r="H1" s="78" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I1" s="78" t="s">
         <v>263</v>
@@ -4600,7 +4569,7 @@
         <v>250</v>
       </c>
       <c r="H2" s="78" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I2" s="78" t="s">
         <v>262</v>
@@ -4633,25 +4602,25 @@
       </c>
       <c r="B3" s="84"/>
       <c r="C3" s="77" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D3" s="87" t="s">
         <v>266</v>
       </c>
       <c r="E3" s="87" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G3" s="77" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H3" s="77" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I3" s="77" t="s">
+        <v>304</v>
+      </c>
+      <c r="J3" s="77" t="s">
         <v>305</v>
-      </c>
-      <c r="J3" s="77" t="s">
-        <v>306</v>
       </c>
       <c r="K3" s="77" t="s">
         <v>237</v>
@@ -4663,16 +4632,16 @@
         <v>264</v>
       </c>
       <c r="N3" s="86" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O3" s="86" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P3" s="86" t="s">
-        <v>268</v>
+        <v>395</v>
       </c>
       <c r="Q3" s="84" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="32.4">
@@ -4686,19 +4655,19 @@
         <v>266</v>
       </c>
       <c r="E4" s="85" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G4" s="77" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H4" s="79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I4" s="77" t="s">
+        <v>304</v>
+      </c>
+      <c r="J4" s="77" t="s">
         <v>305</v>
-      </c>
-      <c r="J4" s="77" t="s">
-        <v>306</v>
       </c>
       <c r="K4" s="79" t="s">
         <v>221</v>
@@ -4710,16 +4679,16 @@
         <v>264</v>
       </c>
       <c r="N4" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O4" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P4" s="80" t="s">
-        <v>268</v>
+        <v>396</v>
       </c>
       <c r="Q4" s="84" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="32.4">
@@ -4733,20 +4702,20 @@
         <v>266</v>
       </c>
       <c r="E5" s="85" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F5" s="81"/>
       <c r="G5" s="77" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I5" s="77" t="s">
+        <v>304</v>
+      </c>
+      <c r="J5" s="77" t="s">
         <v>305</v>
-      </c>
-      <c r="J5" s="77" t="s">
-        <v>306</v>
       </c>
       <c r="K5" s="79" t="s">
         <v>236</v>
@@ -4758,16 +4727,16 @@
         <v>264</v>
       </c>
       <c r="N5" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O5" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P5" s="80" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Q5" s="84" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="32.4">
@@ -4778,23 +4747,23 @@
         <v>218</v>
       </c>
       <c r="D6" s="84" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E6" s="84" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F6" s="51"/>
       <c r="G6" s="77" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H6" s="79" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I6" s="77" t="s">
+        <v>304</v>
+      </c>
+      <c r="J6" s="77" t="s">
         <v>305</v>
-      </c>
-      <c r="J6" s="77" t="s">
-        <v>306</v>
       </c>
       <c r="K6" s="79" t="s">
         <v>221</v>
@@ -4803,19 +4772,19 @@
         <v>239</v>
       </c>
       <c r="M6" s="80" t="s">
+        <v>273</v>
+      </c>
+      <c r="N6" s="80" t="s">
         <v>274</v>
       </c>
-      <c r="N6" s="80" t="s">
+      <c r="O6" s="80" t="s">
+        <v>274</v>
+      </c>
+      <c r="P6" s="93" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q6" s="84" t="s">
         <v>275</v>
-      </c>
-      <c r="O6" s="80" t="s">
-        <v>275</v>
-      </c>
-      <c r="P6" s="93" t="s">
-        <v>338</v>
-      </c>
-      <c r="Q6" s="84" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="32.4">
@@ -4826,23 +4795,23 @@
         <v>232</v>
       </c>
       <c r="D7" s="84" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E7" s="84" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F7" s="81"/>
       <c r="G7" s="77" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H7" s="81" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I7" s="77" t="s">
+        <v>304</v>
+      </c>
+      <c r="J7" s="77" t="s">
         <v>305</v>
-      </c>
-      <c r="J7" s="77" t="s">
-        <v>306</v>
       </c>
       <c r="K7" s="79" t="s">
         <v>236</v>
@@ -4851,19 +4820,19 @@
         <v>239</v>
       </c>
       <c r="M7" s="80" t="s">
+        <v>273</v>
+      </c>
+      <c r="N7" s="80" t="s">
         <v>274</v>
       </c>
-      <c r="N7" s="80" t="s">
-        <v>275</v>
-      </c>
       <c r="O7" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P7" s="80" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Q7" s="84" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -4871,25 +4840,25 @@
         <v>225</v>
       </c>
       <c r="C8" s="82" t="s">
+        <v>318</v>
+      </c>
+      <c r="D8" s="79" t="s">
         <v>319</v>
       </c>
-      <c r="D8" s="79" t="s">
-        <v>320</v>
-      </c>
       <c r="F8" s="82" t="s">
+        <v>321</v>
+      </c>
+      <c r="G8" s="82" t="s">
         <v>322</v>
       </c>
-      <c r="G8" s="82" t="s">
-        <v>323</v>
-      </c>
       <c r="H8" s="82" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I8" s="77" t="s">
+        <v>304</v>
+      </c>
+      <c r="J8" s="77" t="s">
         <v>305</v>
-      </c>
-      <c r="J8" s="77" t="s">
-        <v>306</v>
       </c>
       <c r="K8" s="83" t="s">
         <v>237</v>
@@ -4899,10 +4868,10 @@
       </c>
       <c r="M8" s="80"/>
       <c r="N8" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O8" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P8" s="80"/>
     </row>
@@ -4914,22 +4883,22 @@
         <v>209</v>
       </c>
       <c r="D9" s="79" t="s">
+        <v>320</v>
+      </c>
+      <c r="F9" s="82" t="s">
         <v>321</v>
       </c>
-      <c r="F9" s="82" t="s">
+      <c r="G9" s="82" t="s">
         <v>322</v>
       </c>
-      <c r="G9" s="82" t="s">
-        <v>323</v>
-      </c>
       <c r="H9" s="82" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I9" s="77" t="s">
+        <v>304</v>
+      </c>
+      <c r="J9" s="77" t="s">
         <v>305</v>
-      </c>
-      <c r="J9" s="77" t="s">
-        <v>306</v>
       </c>
       <c r="K9" s="83" t="s">
         <v>237</v>
@@ -4939,10 +4908,10 @@
       </c>
       <c r="M9" s="80"/>
       <c r="N9" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O9" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P9" s="80"/>
     </row>
@@ -4951,32 +4920,32 @@
         <v>227</v>
       </c>
       <c r="C10" s="79" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D10" s="79" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H10" s="79" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I10" s="77" t="s">
+        <v>304</v>
+      </c>
+      <c r="J10" s="77" t="s">
         <v>305</v>
       </c>
-      <c r="J10" s="77" t="s">
-        <v>306</v>
-      </c>
       <c r="K10" s="79" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="L10" s="80" t="s">
         <v>238</v>
       </c>
       <c r="M10" s="80"/>
       <c r="N10" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O10" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P10" s="80"/>
     </row>
@@ -4991,16 +4960,16 @@
         <v>210</v>
       </c>
       <c r="D11" s="79" t="s">
+        <v>333</v>
+      </c>
+      <c r="F11" s="82" t="s">
+        <v>321</v>
+      </c>
+      <c r="G11" s="79" t="s">
         <v>334</v>
       </c>
-      <c r="F11" s="82" t="s">
-        <v>322</v>
-      </c>
-      <c r="G11" s="79" t="s">
+      <c r="H11" s="79" t="s">
         <v>335</v>
-      </c>
-      <c r="H11" s="79" t="s">
-        <v>336</v>
       </c>
       <c r="I11" s="77"/>
       <c r="J11" s="77"/>
@@ -5016,16 +4985,16 @@
         <v>211</v>
       </c>
       <c r="D12" s="79" t="s">
+        <v>333</v>
+      </c>
+      <c r="F12" s="82" t="s">
+        <v>321</v>
+      </c>
+      <c r="G12" s="79" t="s">
         <v>334</v>
       </c>
-      <c r="F12" s="82" t="s">
-        <v>322</v>
-      </c>
-      <c r="G12" s="79" t="s">
+      <c r="H12" s="79" t="s">
         <v>335</v>
-      </c>
-      <c r="H12" s="79" t="s">
-        <v>336</v>
       </c>
       <c r="I12" s="77"/>
       <c r="J12" s="77"/>
@@ -5041,16 +5010,16 @@
         <v>212</v>
       </c>
       <c r="D13" s="79" t="s">
+        <v>333</v>
+      </c>
+      <c r="F13" s="82" t="s">
+        <v>321</v>
+      </c>
+      <c r="G13" s="79" t="s">
         <v>334</v>
       </c>
-      <c r="F13" s="82" t="s">
-        <v>322</v>
-      </c>
-      <c r="G13" s="79" t="s">
+      <c r="H13" s="79" t="s">
         <v>335</v>
-      </c>
-      <c r="H13" s="79" t="s">
-        <v>336</v>
       </c>
       <c r="I13" s="77"/>
       <c r="J13" s="77"/>
@@ -5066,52 +5035,52 @@
         <v>213</v>
       </c>
       <c r="D14" s="79" t="s">
+        <v>333</v>
+      </c>
+      <c r="F14" s="82" t="s">
+        <v>321</v>
+      </c>
+      <c r="G14" s="79" t="s">
         <v>334</v>
       </c>
-      <c r="F14" s="82" t="s">
-        <v>322</v>
-      </c>
-      <c r="G14" s="79" t="s">
+      <c r="H14" s="79" t="s">
         <v>335</v>
-      </c>
-      <c r="H14" s="79" t="s">
-        <v>336</v>
       </c>
       <c r="I14" s="77"/>
       <c r="J14" s="77"/>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="81" t="s">
+        <v>339</v>
+      </c>
+      <c r="C15" s="79" t="s">
         <v>340</v>
-      </c>
-      <c r="C15" s="79" t="s">
-        <v>341</v>
       </c>
       <c r="F15" s="82"/>
       <c r="I15" s="77"/>
       <c r="J15" s="77"/>
       <c r="K15" s="79" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="81" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C16" s="51" t="s">
         <v>214</v>
       </c>
       <c r="D16" s="79" t="s">
+        <v>333</v>
+      </c>
+      <c r="F16" s="82" t="s">
+        <v>321</v>
+      </c>
+      <c r="G16" s="79" t="s">
         <v>334</v>
       </c>
-      <c r="F16" s="82" t="s">
-        <v>322</v>
-      </c>
-      <c r="G16" s="79" t="s">
+      <c r="H16" s="79" t="s">
         <v>335</v>
-      </c>
-      <c r="H16" s="79" t="s">
-        <v>336</v>
       </c>
       <c r="I16" s="77"/>
       <c r="J16" s="77"/>
@@ -5119,22 +5088,22 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="81" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C17" s="51" t="s">
         <v>215</v>
       </c>
       <c r="D17" s="79" t="s">
+        <v>333</v>
+      </c>
+      <c r="F17" s="82" t="s">
+        <v>321</v>
+      </c>
+      <c r="G17" s="79" t="s">
         <v>334</v>
       </c>
-      <c r="F17" s="82" t="s">
-        <v>322</v>
-      </c>
-      <c r="G17" s="79" t="s">
+      <c r="H17" s="79" t="s">
         <v>335</v>
-      </c>
-      <c r="H17" s="79" t="s">
-        <v>336</v>
       </c>
       <c r="I17" s="77"/>
       <c r="J17" s="77"/>
@@ -5142,22 +5111,22 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="81" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C18" s="79" t="s">
         <v>216</v>
       </c>
       <c r="D18" s="79" t="s">
+        <v>333</v>
+      </c>
+      <c r="F18" s="82" t="s">
+        <v>321</v>
+      </c>
+      <c r="G18" s="79" t="s">
         <v>334</v>
       </c>
-      <c r="F18" s="82" t="s">
-        <v>322</v>
-      </c>
-      <c r="G18" s="79" t="s">
+      <c r="H18" s="79" t="s">
         <v>335</v>
-      </c>
-      <c r="H18" s="79" t="s">
-        <v>336</v>
       </c>
       <c r="I18" s="77"/>
       <c r="J18" s="77"/>
@@ -5165,22 +5134,22 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="81" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C19" s="79" t="s">
         <v>217</v>
       </c>
       <c r="D19" s="79" t="s">
+        <v>333</v>
+      </c>
+      <c r="F19" s="82" t="s">
+        <v>321</v>
+      </c>
+      <c r="G19" s="79" t="s">
         <v>334</v>
       </c>
-      <c r="F19" s="82" t="s">
-        <v>322</v>
-      </c>
-      <c r="G19" s="79" t="s">
+      <c r="H19" s="79" t="s">
         <v>335</v>
-      </c>
-      <c r="H19" s="79" t="s">
-        <v>336</v>
       </c>
       <c r="I19" s="77"/>
       <c r="J19" s="77"/>
@@ -5188,44 +5157,44 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="81" t="s">
+        <v>364</v>
+      </c>
+      <c r="C20" s="79" t="s">
         <v>365</v>
       </c>
-      <c r="C20" s="79" t="s">
-        <v>366</v>
-      </c>
       <c r="D20" s="79" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I20" s="77"/>
       <c r="J20" s="77"/>
       <c r="K20" s="79" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="39.6" customHeight="1">
       <c r="A21" s="90" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C21" s="79" t="s">
+        <v>287</v>
+      </c>
+      <c r="D21" s="79" t="s">
+        <v>324</v>
+      </c>
+      <c r="E21" s="79" t="s">
+        <v>348</v>
+      </c>
+      <c r="G21" s="79" t="s">
+        <v>295</v>
+      </c>
+      <c r="H21" s="79" t="s">
         <v>288</v>
       </c>
-      <c r="D21" s="79" t="s">
-        <v>325</v>
-      </c>
-      <c r="E21" s="79" t="s">
-        <v>349</v>
-      </c>
-      <c r="G21" s="79" t="s">
-        <v>296</v>
-      </c>
-      <c r="H21" s="79" t="s">
-        <v>289</v>
-      </c>
       <c r="I21" s="77" t="s">
+        <v>304</v>
+      </c>
+      <c r="J21" s="77" t="s">
         <v>305</v>
-      </c>
-      <c r="J21" s="77" t="s">
-        <v>306</v>
       </c>
       <c r="K21" s="79" t="s">
         <v>236</v>
@@ -5234,30 +5203,30 @@
         <v>239</v>
       </c>
       <c r="N21" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O21" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P21" s="79" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="39.6" customHeight="1">
       <c r="A22" s="92" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C22" s="79" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E22" s="79" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F22" s="79" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G22" s="79" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I22" s="77"/>
       <c r="J22" s="77"/>
@@ -5267,22 +5236,22 @@
     </row>
     <row r="23" spans="1:17" ht="39.6" customHeight="1">
       <c r="A23" s="92" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C23" s="79" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D23" s="79" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E23" s="79" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F23" s="79" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G23" s="79" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I23" s="77"/>
       <c r="J23" s="77"/>
@@ -5299,28 +5268,28 @@
     </row>
     <row r="25" spans="1:17" ht="32.4">
       <c r="A25" s="90" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C25" s="79" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D25" s="84" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E25" s="84" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G25" s="79" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H25" s="79" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I25" s="77" t="s">
+        <v>304</v>
+      </c>
+      <c r="J25" s="77" t="s">
         <v>305</v>
-      </c>
-      <c r="J25" s="77" t="s">
-        <v>306</v>
       </c>
       <c r="K25" s="79" t="s">
         <v>236</v>
@@ -5329,19 +5298,19 @@
         <v>239</v>
       </c>
       <c r="M25" s="79" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N25" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O25" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P25" s="79" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Q25" s="79" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -5354,100 +5323,100 @@
     </row>
     <row r="28" spans="1:17" ht="64.8">
       <c r="A28" s="89" t="s">
+        <v>313</v>
+      </c>
+      <c r="C28" s="84" t="s">
         <v>314</v>
       </c>
-      <c r="C28" s="84" t="s">
-        <v>315</v>
-      </c>
       <c r="D28" s="84" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E28" s="84" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G28" s="77" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H28" s="79" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I28" s="77" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J28" s="77" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K28" s="79" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L28" s="80" t="s">
         <v>239</v>
       </c>
       <c r="M28" s="84" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N28" s="79" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="O28" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P28" s="84" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Q28" s="79" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="55.95" customHeight="1">
       <c r="A29" s="90" t="s">
+        <v>280</v>
+      </c>
+      <c r="C29" s="79" t="s">
         <v>281</v>
       </c>
-      <c r="C29" s="79" t="s">
-        <v>282</v>
-      </c>
       <c r="D29" s="84" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E29" s="84" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G29" s="77" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H29" s="79" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I29" s="77" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J29" s="77" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K29" s="79" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L29" s="80" t="s">
         <v>239</v>
       </c>
       <c r="M29" s="84" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="N29" s="79" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="O29" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P29" s="84" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q29" s="79" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q1" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A1:Q1"/>
   <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>